<commit_message>
TAKEN 1 & 2
</commit_message>
<xml_diff>
--- a/MVandebroek/TAKEN/TASK0/1. FILES/archive/responses_test_TAAK0.xlsx
+++ b/MVandebroek/TAKEN/TASK0/1. FILES/archive/responses_test_TAAK0.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0118298\OneDrive\Projects\MVandebroek\TAKEN\TASK0\1. FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25F7082C-BBF6-44D8-A073-C11C2BD719B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D09B0BBE-50F1-486A-8347-1E74E8A74A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="2904" yWindow="3252" windowWidth="19320" windowHeight="7212"/>
   </bookViews>
   <sheets>
-    <sheet name="responses_test_TAAK0" sheetId="1" r:id="rId1"/>
+    <sheet name="TASK0-116082023.downloadlong (1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -929,9 +929,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="130.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>